<commit_message>
Adicionando fotos de novos produtos
</commit_message>
<xml_diff>
--- a/loja.xlsx
+++ b/loja.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projetos_Phayton\Primeiro_Projeto_Pedidos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6C19C32-1E8B-466D-B090-59656DC70A9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E82D1713-6B59-498D-9F73-03BCE4FC376D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{FBB427EC-10B9-4DA4-9183-90BA09539D31}"/>
   </bookViews>
@@ -44,9 +44,6 @@
     <t>PREZ CATUMBI</t>
   </si>
   <si>
-    <t>SENADOR CAMARA</t>
-  </si>
-  <si>
     <t>PREZ BENFICA</t>
   </si>
   <si>
@@ -86,9 +83,6 @@
     <t>PREZ CAMPINHO</t>
   </si>
   <si>
-    <t xml:space="preserve"> PREZ TAQUARA</t>
-  </si>
-  <si>
     <t>PREZ ITAOCA</t>
   </si>
   <si>
@@ -140,55 +134,61 @@
     <t>PREZUNIC MARICA</t>
   </si>
   <si>
-    <t>ASSAI ILHA - 29</t>
-  </si>
-  <si>
-    <t>ASSAI CABO FRIO - 82</t>
-  </si>
-  <si>
-    <t>ASSAI CAXIAS - 131</t>
-  </si>
-  <si>
-    <t>ASSAI MESQUITA 142</t>
-  </si>
-  <si>
-    <t>ASSAI TIJUCA 2 - 150</t>
-  </si>
-  <si>
     <t>ASSAI MEIER</t>
   </si>
   <si>
-    <t>ASSAI PETROPOLIS - 181</t>
-  </si>
-  <si>
-    <t>ASSAI SANTA CRUZ - 202</t>
-  </si>
-  <si>
-    <t>ASSAI (CESARIO DE MELLO) 202</t>
-  </si>
-  <si>
-    <t>ASSAI MACAÉ - 232</t>
-  </si>
-  <si>
-    <t>ASSAI BARRA 2 - 245</t>
-  </si>
-  <si>
-    <t>TRIBOBÓ - 248</t>
-  </si>
-  <si>
-    <t>ASSAI MARACANA - 286</t>
-  </si>
-  <si>
     <t>ASSAI GALEAO</t>
   </si>
   <si>
-    <t>CARIOCA - 316</t>
-  </si>
-  <si>
     <t>numero</t>
   </si>
   <si>
     <t>loja</t>
+  </si>
+  <si>
+    <t>PREZ TAQUARA</t>
+  </si>
+  <si>
+    <t>ASSAI CARIOCA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ASSAI TRIBOBÓ </t>
+  </si>
+  <si>
+    <t>ASSAI TIJUCA 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ASSAI SANTA CRUZ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ASSAI PETROPOLIS </t>
+  </si>
+  <si>
+    <t>ASSAI MESQUITA</t>
+  </si>
+  <si>
+    <t>ASSAI MARACANA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ASSAI MACAÉ </t>
+  </si>
+  <si>
+    <t>ASSAI ILHA</t>
+  </si>
+  <si>
+    <t>ASSAI CAXIAS</t>
+  </si>
+  <si>
+    <t>ASSAI CABO FRIO</t>
+  </si>
+  <si>
+    <t>ASSAI BARRA 2</t>
+  </si>
+  <si>
+    <t>ASSAI CESARIO DE MELLO</t>
+  </si>
+  <si>
+    <t>PREZUNIC SENADOR CAMARA</t>
   </si>
 </sst>
 </file>
@@ -376,9 +376,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office 2013 - 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -416,7 +416,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -522,7 +522,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -664,7 +664,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -675,7 +675,7 @@
   <dimension ref="A1:B50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -686,405 +686,408 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1">
-        <v>702</v>
+        <v>202</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>0</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1">
-        <v>704</v>
+        <v>245</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>1</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1">
-        <v>705</v>
+        <v>82</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>2</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1">
-        <v>706</v>
+        <v>131</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>3</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1">
-        <v>707</v>
+        <v>302</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1">
-        <v>708</v>
+        <v>29</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>5</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1">
-        <v>709</v>
+        <v>232</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>6</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1">
-        <v>710</v>
+        <v>286</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1">
-        <v>711</v>
+        <v>160</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="1">
-        <v>712</v>
+        <v>142</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>9</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="1">
-        <v>713</v>
+        <v>181</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="1">
-        <v>714</v>
+        <v>201</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1">
-        <v>715</v>
+        <v>150</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>12</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="1">
-        <v>716</v>
+        <v>248</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>13</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="1">
-        <v>717</v>
+        <v>316</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>14</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="1">
-        <v>718</v>
+        <v>714</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="1">
-        <v>719</v>
+        <v>723</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="1">
-        <v>720</v>
+        <v>734</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="1">
-        <v>721</v>
+        <v>706</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="1">
-        <v>722</v>
+        <v>731</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="1">
-        <v>723</v>
+        <v>724</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="1">
-        <v>724</v>
+        <v>713</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="1">
-        <v>725</v>
+        <v>718</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="1">
-        <v>726</v>
+        <v>704</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>23</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="1">
-        <v>728</v>
+        <v>717</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="1">
-        <v>729</v>
+        <v>716</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="1">
-        <v>730</v>
+        <v>710</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="1">
-        <v>731</v>
+        <v>708</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>27</v>
+        <v>4</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="1">
-        <v>733</v>
+        <v>722</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="1">
-        <v>734</v>
+        <v>707</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>29</v>
+        <v>3</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" s="1">
-        <v>736</v>
+        <v>730</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="1">
-        <v>747</v>
+        <v>728</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="1">
-        <v>742</v>
+        <v>720</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="1">
-        <v>745</v>
+        <v>711</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" s="1">
-        <v>29</v>
+        <v>729</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="1">
-        <v>82</v>
+        <v>721</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="1">
-        <v>131</v>
+        <v>726</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" s="1">
-        <v>142</v>
+        <v>736</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" s="1">
-        <v>150</v>
+        <v>709</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>38</v>
+        <v>5</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" s="1">
-        <v>160</v>
+        <v>712</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="1">
-        <v>181</v>
+        <v>702</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>40</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" s="1">
-        <v>201</v>
+        <v>733</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" s="1">
-        <v>202</v>
+        <v>719</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" s="1">
-        <v>232</v>
+        <v>725</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>43</v>
+        <v>20</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" s="1">
-        <v>245</v>
+        <v>715</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" s="1">
-        <v>248</v>
+        <v>747</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" s="1">
-        <v>286</v>
+        <v>745</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" s="1">
-        <v>302</v>
+        <v>742</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" s="1">
-        <v>316</v>
+        <v>705</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B50">
+    <sortCondition ref="B2:B50"/>
+  </sortState>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>